<commit_message>
advance report with excel
</commit_message>
<xml_diff>
--- a/public/templates/report_template.xlsx
+++ b/public/templates/report_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcastillo\Documents\QuisVar\quisvar_proyect_ft\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E577CF05-EE3E-4ADD-BAC6-A47099663E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F9B268-C4AB-48EA-9955-59EE1D0E6EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="482" firstSheet="1" activeTab="1" xr2:uid="{F98A2DB2-54A5-485C-A701-CE43CF6B2BAF}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="395">
   <si>
     <t>ITEM</t>
   </si>
@@ -1726,9 +1726,6 @@
   </si>
   <si>
     <t>28 DE MARZO del 2023</t>
-  </si>
-  <si>
-    <t>al 16 de marzo del 2023</t>
   </si>
   <si>
     <t>INFORME PARCIAL DE SERVICIOS PROFESIONALES PRESTADOS COMO COORDINADOR DEL AREA SANITARIAS DE PROYECTOS</t>
@@ -3172,7 +3169,7 @@
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="334">
+  <cellXfs count="333">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3777,6 +3774,12 @@
     <xf numFmtId="164" fontId="41" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3909,12 +3912,6 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="23" fillId="9" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="38" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3987,9 +3984,6 @@
     <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="167" fontId="25" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4080,8 +4074,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -4465,174 +4459,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="247" t="s">
+      <c r="A1" s="249" t="s">
         <v>335</v>
       </c>
-      <c r="B1" s="246"/>
-      <c r="C1" s="246"/>
-      <c r="D1" s="246"/>
-      <c r="E1" s="246"/>
-      <c r="F1" s="246"/>
-      <c r="G1" s="246"/>
-      <c r="H1" s="246"/>
-      <c r="I1" s="246"/>
-      <c r="J1" s="246"/>
-      <c r="K1" s="246"/>
-      <c r="L1" s="246"/>
-      <c r="M1" s="246"/>
-      <c r="N1" s="246"/>
-      <c r="O1" s="245" t="s">
+      <c r="B1" s="248"/>
+      <c r="C1" s="248"/>
+      <c r="D1" s="248"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
+      <c r="G1" s="248"/>
+      <c r="H1" s="248"/>
+      <c r="I1" s="248"/>
+      <c r="J1" s="248"/>
+      <c r="K1" s="248"/>
+      <c r="L1" s="248"/>
+      <c r="M1" s="248"/>
+      <c r="N1" s="248"/>
+      <c r="O1" s="247" t="s">
         <v>333</v>
       </c>
-      <c r="P1" s="245"/>
-      <c r="Q1" s="245"/>
-      <c r="R1" s="245"/>
-      <c r="S1" s="245"/>
-      <c r="T1" s="245"/>
-      <c r="U1" s="245"/>
-      <c r="V1" s="245"/>
-      <c r="W1" s="245"/>
-      <c r="X1" s="245"/>
-      <c r="Y1" s="245"/>
-      <c r="Z1" s="245"/>
-      <c r="AA1" s="245"/>
-      <c r="AB1" s="245"/>
-      <c r="AC1" s="245"/>
-      <c r="AD1" s="245"/>
-      <c r="AE1" s="245"/>
-      <c r="AF1" s="245"/>
-      <c r="AG1" s="245"/>
-      <c r="AH1" s="246" t="s">
+      <c r="P1" s="247"/>
+      <c r="Q1" s="247"/>
+      <c r="R1" s="247"/>
+      <c r="S1" s="247"/>
+      <c r="T1" s="247"/>
+      <c r="U1" s="247"/>
+      <c r="V1" s="247"/>
+      <c r="W1" s="247"/>
+      <c r="X1" s="247"/>
+      <c r="Y1" s="247"/>
+      <c r="Z1" s="247"/>
+      <c r="AA1" s="247"/>
+      <c r="AB1" s="247"/>
+      <c r="AC1" s="247"/>
+      <c r="AD1" s="247"/>
+      <c r="AE1" s="247"/>
+      <c r="AF1" s="247"/>
+      <c r="AG1" s="247"/>
+      <c r="AH1" s="248" t="s">
         <v>327</v>
       </c>
-      <c r="AI1" s="246"/>
-      <c r="AJ1" s="246"/>
-      <c r="AK1" s="246"/>
-      <c r="AL1" s="243" t="s">
+      <c r="AI1" s="248"/>
+      <c r="AJ1" s="248"/>
+      <c r="AK1" s="248"/>
+      <c r="AL1" s="245" t="s">
         <v>334</v>
       </c>
-      <c r="AM1" s="243"/>
-      <c r="AN1" s="243"/>
-      <c r="AO1" s="243"/>
-      <c r="AP1" s="243"/>
-      <c r="AQ1" s="243"/>
-      <c r="AR1" s="243"/>
-      <c r="AS1" s="243"/>
-      <c r="AT1" s="243"/>
-      <c r="AU1" s="243"/>
-      <c r="AV1" s="243"/>
-      <c r="AW1" s="243"/>
-      <c r="AX1" s="243"/>
-      <c r="AY1" s="243"/>
-      <c r="AZ1" s="243"/>
-      <c r="BA1" s="243"/>
-      <c r="BB1" s="243"/>
-      <c r="BC1" s="243"/>
-      <c r="BD1" s="244"/>
+      <c r="AM1" s="245"/>
+      <c r="AN1" s="245"/>
+      <c r="AO1" s="245"/>
+      <c r="AP1" s="245"/>
+      <c r="AQ1" s="245"/>
+      <c r="AR1" s="245"/>
+      <c r="AS1" s="245"/>
+      <c r="AT1" s="245"/>
+      <c r="AU1" s="245"/>
+      <c r="AV1" s="245"/>
+      <c r="AW1" s="245"/>
+      <c r="AX1" s="245"/>
+      <c r="AY1" s="245"/>
+      <c r="AZ1" s="245"/>
+      <c r="BA1" s="245"/>
+      <c r="BB1" s="245"/>
+      <c r="BC1" s="245"/>
+      <c r="BD1" s="246"/>
     </row>
     <row r="2" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="266" t="s">
+      <c r="A2" s="268" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="267"/>
+      <c r="B2" s="269"/>
       <c r="C2" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D2" s="270" t="s">
+      <c r="D2" s="272" t="s">
         <v>337</v>
       </c>
-      <c r="E2" s="270"/>
-      <c r="F2" s="235" t="s">
+      <c r="E2" s="272"/>
+      <c r="F2" s="237" t="s">
         <v>336</v>
       </c>
-      <c r="G2" s="235"/>
-      <c r="H2" s="235"/>
-      <c r="I2" s="235"/>
-      <c r="J2" s="235"/>
-      <c r="K2" s="235"/>
-      <c r="L2" s="235"/>
-      <c r="M2" s="235"/>
-      <c r="N2" s="235"/>
-      <c r="O2" s="235"/>
-      <c r="P2" s="235"/>
-      <c r="Q2" s="235"/>
-      <c r="R2" s="235"/>
-      <c r="S2" s="235"/>
-      <c r="T2" s="235"/>
-      <c r="U2" s="235"/>
-      <c r="V2" s="235"/>
-      <c r="W2" s="235"/>
-      <c r="X2" s="235"/>
-      <c r="Y2" s="235"/>
-      <c r="Z2" s="235"/>
-      <c r="AA2" s="235"/>
-      <c r="AB2" s="235"/>
-      <c r="AC2" s="235"/>
-      <c r="AD2" s="235"/>
-      <c r="AE2" s="235"/>
-      <c r="AF2" s="235"/>
-      <c r="AG2" s="235"/>
-      <c r="AH2" s="235"/>
-      <c r="AI2" s="235"/>
-      <c r="AJ2" s="235"/>
-      <c r="AK2" s="235"/>
-      <c r="AL2" s="235"/>
-      <c r="AM2" s="235"/>
-      <c r="AN2" s="235"/>
-      <c r="AO2" s="235"/>
-      <c r="AP2" s="235"/>
-      <c r="AQ2" s="235"/>
-      <c r="AR2" s="235"/>
-      <c r="AS2" s="235"/>
-      <c r="AT2" s="235"/>
-      <c r="AU2" s="235"/>
-      <c r="AV2" s="235"/>
-      <c r="AW2" s="235"/>
-      <c r="AX2" s="235"/>
-      <c r="AY2" s="235"/>
-      <c r="AZ2" s="235"/>
-      <c r="BA2" s="235"/>
-      <c r="BB2" s="235"/>
-      <c r="BC2" s="235"/>
-      <c r="BD2" s="236"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="237"/>
+      <c r="I2" s="237"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237"/>
+      <c r="L2" s="237"/>
+      <c r="M2" s="237"/>
+      <c r="N2" s="237"/>
+      <c r="O2" s="237"/>
+      <c r="P2" s="237"/>
+      <c r="Q2" s="237"/>
+      <c r="R2" s="237"/>
+      <c r="S2" s="237"/>
+      <c r="T2" s="237"/>
+      <c r="U2" s="237"/>
+      <c r="V2" s="237"/>
+      <c r="W2" s="237"/>
+      <c r="X2" s="237"/>
+      <c r="Y2" s="237"/>
+      <c r="Z2" s="237"/>
+      <c r="AA2" s="237"/>
+      <c r="AB2" s="237"/>
+      <c r="AC2" s="237"/>
+      <c r="AD2" s="237"/>
+      <c r="AE2" s="237"/>
+      <c r="AF2" s="237"/>
+      <c r="AG2" s="237"/>
+      <c r="AH2" s="237"/>
+      <c r="AI2" s="237"/>
+      <c r="AJ2" s="237"/>
+      <c r="AK2" s="237"/>
+      <c r="AL2" s="237"/>
+      <c r="AM2" s="237"/>
+      <c r="AN2" s="237"/>
+      <c r="AO2" s="237"/>
+      <c r="AP2" s="237"/>
+      <c r="AQ2" s="237"/>
+      <c r="AR2" s="237"/>
+      <c r="AS2" s="237"/>
+      <c r="AT2" s="237"/>
+      <c r="AU2" s="237"/>
+      <c r="AV2" s="237"/>
+      <c r="AW2" s="237"/>
+      <c r="AX2" s="237"/>
+      <c r="AY2" s="237"/>
+      <c r="AZ2" s="237"/>
+      <c r="BA2" s="237"/>
+      <c r="BB2" s="237"/>
+      <c r="BC2" s="237"/>
+      <c r="BD2" s="238"/>
     </row>
     <row r="3" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="266" t="s">
+      <c r="A3" s="268" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="267"/>
+      <c r="B3" s="269"/>
       <c r="C3" s="141" t="s">
         <v>286</v>
       </c>
-      <c r="D3" s="249" t="s">
+      <c r="D3" s="251" t="s">
         <v>338</v>
       </c>
-      <c r="E3" s="249"/>
+      <c r="E3" s="251"/>
       <c r="F3" s="145">
         <v>75263586</v>
       </c>
       <c r="G3" s="145"/>
       <c r="H3" s="145"/>
-      <c r="I3" s="249" t="s">
+      <c r="I3" s="251" t="s">
         <v>342</v>
       </c>
-      <c r="J3" s="249"/>
-      <c r="K3" s="249"/>
-      <c r="L3" s="249"/>
-      <c r="M3" s="249"/>
-      <c r="N3" s="249"/>
-      <c r="O3" s="249"/>
-      <c r="P3" s="249"/>
-      <c r="Q3" s="249"/>
-      <c r="R3" s="238" t="s">
+      <c r="J3" s="251"/>
+      <c r="K3" s="251"/>
+      <c r="L3" s="251"/>
+      <c r="M3" s="251"/>
+      <c r="N3" s="251"/>
+      <c r="O3" s="251"/>
+      <c r="P3" s="251"/>
+      <c r="Q3" s="251"/>
+      <c r="R3" s="240" t="s">
         <v>344</v>
       </c>
-      <c r="S3" s="238"/>
-      <c r="T3" s="238"/>
-      <c r="U3" s="238"/>
-      <c r="V3" s="238"/>
-      <c r="W3" s="238"/>
-      <c r="X3" s="238"/>
+      <c r="S3" s="240"/>
+      <c r="T3" s="240"/>
+      <c r="U3" s="240"/>
+      <c r="V3" s="240"/>
+      <c r="W3" s="240"/>
+      <c r="X3" s="240"/>
       <c r="Y3" s="143"/>
       <c r="Z3" s="143"/>
       <c r="AA3" s="143"/>
@@ -4667,42 +4661,42 @@
       <c r="BD3" s="139"/>
     </row>
     <row r="4" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="266" t="s">
+      <c r="A4" s="268" t="s">
         <v>296</v>
       </c>
-      <c r="B4" s="267"/>
+      <c r="B4" s="269"/>
       <c r="C4" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D4" s="249" t="s">
+      <c r="D4" s="251" t="s">
         <v>339</v>
       </c>
-      <c r="E4" s="249"/>
+      <c r="E4" s="251"/>
       <c r="F4" s="145">
         <v>99826036</v>
       </c>
       <c r="G4" s="145"/>
       <c r="H4" s="145"/>
-      <c r="I4" s="249" t="s">
+      <c r="I4" s="251" t="s">
         <v>343</v>
       </c>
-      <c r="J4" s="249"/>
-      <c r="K4" s="249"/>
-      <c r="L4" s="249"/>
-      <c r="M4" s="249"/>
-      <c r="N4" s="249"/>
-      <c r="O4" s="249"/>
-      <c r="P4" s="249"/>
-      <c r="Q4" s="249"/>
-      <c r="R4" s="238" t="s">
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="251"/>
+      <c r="M4" s="251"/>
+      <c r="N4" s="251"/>
+      <c r="O4" s="251"/>
+      <c r="P4" s="251"/>
+      <c r="Q4" s="251"/>
+      <c r="R4" s="240" t="s">
         <v>345</v>
       </c>
-      <c r="S4" s="238"/>
-      <c r="T4" s="238"/>
-      <c r="U4" s="238"/>
-      <c r="V4" s="238"/>
-      <c r="W4" s="238"/>
-      <c r="X4" s="238"/>
+      <c r="S4" s="240"/>
+      <c r="T4" s="240"/>
+      <c r="U4" s="240"/>
+      <c r="V4" s="240"/>
+      <c r="W4" s="240"/>
+      <c r="X4" s="240"/>
       <c r="Y4" s="143"/>
       <c r="Z4" s="143"/>
       <c r="AA4" s="143"/>
@@ -4737,35 +4731,35 @@
       <c r="BD4" s="139"/>
     </row>
     <row r="5" spans="1:56" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="268" t="s">
+      <c r="A5" s="270" t="s">
         <v>309</v>
       </c>
-      <c r="B5" s="269"/>
+      <c r="B5" s="271"/>
       <c r="C5" s="142" t="s">
         <v>288</v>
       </c>
-      <c r="D5" s="271" t="s">
+      <c r="D5" s="273" t="s">
         <v>340</v>
       </c>
-      <c r="E5" s="271"/>
-      <c r="F5" s="237" t="s">
+      <c r="E5" s="273"/>
+      <c r="F5" s="239" t="s">
         <v>341</v>
       </c>
-      <c r="G5" s="237"/>
-      <c r="H5" s="237"/>
-      <c r="I5" s="237"/>
-      <c r="J5" s="237"/>
-      <c r="K5" s="237"/>
-      <c r="L5" s="237"/>
-      <c r="M5" s="237"/>
-      <c r="N5" s="237"/>
-      <c r="O5" s="237"/>
-      <c r="P5" s="237"/>
-      <c r="Q5" s="237"/>
-      <c r="R5" s="237"/>
-      <c r="S5" s="237"/>
-      <c r="T5" s="237"/>
-      <c r="U5" s="237"/>
+      <c r="G5" s="239"/>
+      <c r="H5" s="239"/>
+      <c r="I5" s="239"/>
+      <c r="J5" s="239"/>
+      <c r="K5" s="239"/>
+      <c r="L5" s="239"/>
+      <c r="M5" s="239"/>
+      <c r="N5" s="239"/>
+      <c r="O5" s="239"/>
+      <c r="P5" s="239"/>
+      <c r="Q5" s="239"/>
+      <c r="R5" s="239"/>
+      <c r="S5" s="239"/>
+      <c r="T5" s="239"/>
+      <c r="U5" s="239"/>
       <c r="V5" s="144"/>
       <c r="W5" s="144"/>
       <c r="X5" s="144"/>
@@ -4803,101 +4797,101 @@
       <c r="BD5" s="140"/>
     </row>
     <row r="6" spans="1:56" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="258" t="s">
+      <c r="A6" s="260" t="s">
         <v>320</v>
       </c>
-      <c r="B6" s="260" t="s">
+      <c r="B6" s="262" t="s">
         <v>160</v>
       </c>
-      <c r="C6" s="260" t="s">
+      <c r="C6" s="262" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="260" t="s">
+      <c r="D6" s="262" t="s">
         <v>292</v>
       </c>
-      <c r="E6" s="264" t="s">
+      <c r="E6" s="266" t="s">
         <v>159</v>
       </c>
-      <c r="F6" s="265"/>
-      <c r="G6" s="262" t="s">
+      <c r="F6" s="267"/>
+      <c r="G6" s="264" t="s">
         <v>293</v>
       </c>
-      <c r="H6" s="240" t="s">
+      <c r="H6" s="242" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="241"/>
-      <c r="J6" s="241"/>
-      <c r="K6" s="241"/>
-      <c r="L6" s="241"/>
-      <c r="M6" s="241"/>
-      <c r="N6" s="242"/>
-      <c r="O6" s="240" t="s">
+      <c r="I6" s="243"/>
+      <c r="J6" s="243"/>
+      <c r="K6" s="243"/>
+      <c r="L6" s="243"/>
+      <c r="M6" s="243"/>
+      <c r="N6" s="244"/>
+      <c r="O6" s="242" t="s">
         <v>136</v>
       </c>
-      <c r="P6" s="241"/>
-      <c r="Q6" s="241"/>
-      <c r="R6" s="241"/>
-      <c r="S6" s="241"/>
-      <c r="T6" s="241"/>
-      <c r="U6" s="242"/>
-      <c r="V6" s="240" t="s">
+      <c r="P6" s="243"/>
+      <c r="Q6" s="243"/>
+      <c r="R6" s="243"/>
+      <c r="S6" s="243"/>
+      <c r="T6" s="243"/>
+      <c r="U6" s="244"/>
+      <c r="V6" s="242" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="241"/>
-      <c r="X6" s="241"/>
-      <c r="Y6" s="241"/>
-      <c r="Z6" s="241"/>
-      <c r="AA6" s="241"/>
-      <c r="AB6" s="242"/>
-      <c r="AC6" s="240" t="s">
+      <c r="W6" s="243"/>
+      <c r="X6" s="243"/>
+      <c r="Y6" s="243"/>
+      <c r="Z6" s="243"/>
+      <c r="AA6" s="243"/>
+      <c r="AB6" s="244"/>
+      <c r="AC6" s="242" t="s">
         <v>137</v>
       </c>
-      <c r="AD6" s="241"/>
-      <c r="AE6" s="241"/>
-      <c r="AF6" s="241"/>
-      <c r="AG6" s="241"/>
-      <c r="AH6" s="241"/>
-      <c r="AI6" s="242"/>
-      <c r="AJ6" s="240" t="s">
+      <c r="AD6" s="243"/>
+      <c r="AE6" s="243"/>
+      <c r="AF6" s="243"/>
+      <c r="AG6" s="243"/>
+      <c r="AH6" s="243"/>
+      <c r="AI6" s="244"/>
+      <c r="AJ6" s="242" t="s">
         <v>84</v>
       </c>
-      <c r="AK6" s="241"/>
-      <c r="AL6" s="241"/>
-      <c r="AM6" s="241"/>
-      <c r="AN6" s="241"/>
-      <c r="AO6" s="241"/>
-      <c r="AP6" s="242"/>
-      <c r="AQ6" s="240" t="s">
+      <c r="AK6" s="243"/>
+      <c r="AL6" s="243"/>
+      <c r="AM6" s="243"/>
+      <c r="AN6" s="243"/>
+      <c r="AO6" s="243"/>
+      <c r="AP6" s="244"/>
+      <c r="AQ6" s="242" t="s">
         <v>138</v>
       </c>
-      <c r="AR6" s="241"/>
-      <c r="AS6" s="241"/>
-      <c r="AT6" s="241"/>
-      <c r="AU6" s="241"/>
-      <c r="AV6" s="241"/>
-      <c r="AW6" s="242"/>
-      <c r="AX6" s="240" t="s">
+      <c r="AR6" s="243"/>
+      <c r="AS6" s="243"/>
+      <c r="AT6" s="243"/>
+      <c r="AU6" s="243"/>
+      <c r="AV6" s="243"/>
+      <c r="AW6" s="244"/>
+      <c r="AX6" s="242" t="s">
         <v>139</v>
       </c>
-      <c r="AY6" s="241"/>
-      <c r="AZ6" s="241"/>
-      <c r="BA6" s="241"/>
-      <c r="BB6" s="241"/>
-      <c r="BC6" s="241"/>
-      <c r="BD6" s="242"/>
+      <c r="AY6" s="243"/>
+      <c r="AZ6" s="243"/>
+      <c r="BA6" s="243"/>
+      <c r="BB6" s="243"/>
+      <c r="BC6" s="243"/>
+      <c r="BD6" s="244"/>
     </row>
     <row r="7" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="259"/>
-      <c r="B7" s="261"/>
-      <c r="C7" s="261"/>
-      <c r="D7" s="261"/>
+      <c r="A7" s="261"/>
+      <c r="B7" s="263"/>
+      <c r="C7" s="263"/>
+      <c r="D7" s="263"/>
       <c r="E7" s="154" t="s">
         <v>158</v>
       </c>
       <c r="F7" s="154" t="s">
         <v>319</v>
       </c>
-      <c r="G7" s="263"/>
+      <c r="G7" s="265"/>
       <c r="H7" s="155" t="s">
         <v>297</v>
       </c>
@@ -5171,7 +5165,7 @@
       <c r="BD9" s="89"/>
     </row>
     <row r="10" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="254" t="s">
+      <c r="A10" s="256" t="s">
         <v>321</v>
       </c>
       <c r="B10" s="135"/>
@@ -5239,7 +5233,7 @@
       <c r="BD10" s="89"/>
     </row>
     <row r="11" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="255"/>
+      <c r="A11" s="257"/>
       <c r="B11" s="135"/>
       <c r="C11" s="90" t="s">
         <v>291</v>
@@ -5305,7 +5299,7 @@
       <c r="BD11" s="89"/>
     </row>
     <row r="12" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="257"/>
+      <c r="A12" s="259"/>
       <c r="B12" s="135"/>
       <c r="C12" s="90" t="s">
         <v>89</v>
@@ -5495,7 +5489,7 @@
       <c r="BD14" s="89"/>
     </row>
     <row r="15" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="254" t="s">
+      <c r="A15" s="256" t="s">
         <v>322</v>
       </c>
       <c r="B15" s="135"/>
@@ -5565,7 +5559,7 @@
       <c r="BD15" s="89"/>
     </row>
     <row r="16" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="255"/>
+      <c r="A16" s="257"/>
       <c r="B16" s="135"/>
       <c r="C16" s="95" t="s">
         <v>104</v>
@@ -5633,7 +5627,7 @@
       <c r="BD16" s="89"/>
     </row>
     <row r="17" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="255"/>
+      <c r="A17" s="257"/>
       <c r="B17" s="135"/>
       <c r="C17" s="95" t="s">
         <v>105</v>
@@ -5701,7 +5695,7 @@
       <c r="BD17" s="89"/>
     </row>
     <row r="18" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="255"/>
+      <c r="A18" s="257"/>
       <c r="B18" s="135"/>
       <c r="C18" s="95" t="s">
         <v>106</v>
@@ -5769,7 +5763,7 @@
       <c r="BD18" s="89"/>
     </row>
     <row r="19" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="255"/>
+      <c r="A19" s="257"/>
       <c r="B19" s="135"/>
       <c r="C19" s="95" t="s">
         <v>99</v>
@@ -5837,7 +5831,7 @@
       <c r="BD19" s="89"/>
     </row>
     <row r="20" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="255"/>
+      <c r="A20" s="257"/>
       <c r="B20" s="135"/>
       <c r="C20" s="95" t="s">
         <v>107</v>
@@ -5905,7 +5899,7 @@
       <c r="BD20" s="89"/>
     </row>
     <row r="21" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="255"/>
+      <c r="A21" s="257"/>
       <c r="B21" s="135"/>
       <c r="C21" s="95" t="s">
         <v>108</v>
@@ -5973,7 +5967,7 @@
       <c r="BD21" s="89"/>
     </row>
     <row r="22" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="255"/>
+      <c r="A22" s="257"/>
       <c r="B22" s="135"/>
       <c r="C22" s="95" t="s">
         <v>109</v>
@@ -6041,7 +6035,7 @@
       <c r="BD22" s="89"/>
     </row>
     <row r="23" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="255"/>
+      <c r="A23" s="257"/>
       <c r="B23" s="135"/>
       <c r="C23" s="95" t="s">
         <v>110</v>
@@ -6109,7 +6103,7 @@
       <c r="BD23" s="89"/>
     </row>
     <row r="24" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="255"/>
+      <c r="A24" s="257"/>
       <c r="B24" s="135"/>
       <c r="C24" s="95" t="s">
         <v>111</v>
@@ -6177,7 +6171,7 @@
       <c r="BD24" s="89"/>
     </row>
     <row r="25" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="255"/>
+      <c r="A25" s="257"/>
       <c r="B25" s="135"/>
       <c r="C25" s="95" t="s">
         <v>112</v>
@@ -6245,7 +6239,7 @@
       <c r="BD25" s="89"/>
     </row>
     <row r="26" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="255"/>
+      <c r="A26" s="257"/>
       <c r="B26" s="135"/>
       <c r="C26" s="95" t="s">
         <v>113</v>
@@ -6313,7 +6307,7 @@
       <c r="BD26" s="89"/>
     </row>
     <row r="27" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="255"/>
+      <c r="A27" s="257"/>
       <c r="B27" s="135"/>
       <c r="C27" s="95" t="s">
         <v>114</v>
@@ -6381,7 +6375,7 @@
       <c r="BD27" s="89"/>
     </row>
     <row r="28" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="255"/>
+      <c r="A28" s="257"/>
       <c r="B28" s="135"/>
       <c r="C28" s="95" t="s">
         <v>115</v>
@@ -6449,7 +6443,7 @@
       <c r="BD28" s="89"/>
     </row>
     <row r="29" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="255"/>
+      <c r="A29" s="257"/>
       <c r="B29" s="135"/>
       <c r="C29" s="95" t="s">
         <v>116</v>
@@ -6517,7 +6511,7 @@
       <c r="BD29" s="89"/>
     </row>
     <row r="30" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="257"/>
+      <c r="A30" s="259"/>
       <c r="B30" s="135"/>
       <c r="C30" s="95" t="s">
         <v>117</v>
@@ -6647,7 +6641,7 @@
       <c r="BD31" s="89"/>
     </row>
     <row r="32" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="254" t="s">
+      <c r="A32" s="256" t="s">
         <v>323</v>
       </c>
       <c r="B32" s="135"/>
@@ -6715,7 +6709,7 @@
       <c r="BD32" s="89"/>
     </row>
     <row r="33" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="255"/>
+      <c r="A33" s="257"/>
       <c r="B33" s="135"/>
       <c r="C33" s="95" t="s">
         <v>105</v>
@@ -6781,7 +6775,7 @@
       <c r="BD33" s="89"/>
     </row>
     <row r="34" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="255"/>
+      <c r="A34" s="257"/>
       <c r="B34" s="135"/>
       <c r="C34" s="95" t="s">
         <v>108</v>
@@ -6847,7 +6841,7 @@
       <c r="BD34" s="89"/>
     </row>
     <row r="35" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="257"/>
+      <c r="A35" s="259"/>
       <c r="B35" s="135"/>
       <c r="C35" s="95" t="s">
         <v>91</v>
@@ -6975,7 +6969,7 @@
       <c r="BD36" s="89"/>
     </row>
     <row r="37" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="254" t="s">
+      <c r="A37" s="256" t="s">
         <v>324</v>
       </c>
       <c r="B37" s="136" t="s">
@@ -7039,7 +7033,7 @@
       <c r="BD37" s="89"/>
     </row>
     <row r="38" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="255"/>
+      <c r="A38" s="257"/>
       <c r="B38" s="137" t="s">
         <v>164</v>
       </c>
@@ -7107,7 +7101,7 @@
       <c r="BD38" s="89"/>
     </row>
     <row r="39" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="255"/>
+      <c r="A39" s="257"/>
       <c r="B39" s="137" t="s">
         <v>165</v>
       </c>
@@ -7175,7 +7169,7 @@
       <c r="BD39" s="89"/>
     </row>
     <row r="40" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="255"/>
+      <c r="A40" s="257"/>
       <c r="B40" s="136" t="s">
         <v>225</v>
       </c>
@@ -7237,7 +7231,7 @@
       <c r="BD40" s="89"/>
     </row>
     <row r="41" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="255"/>
+      <c r="A41" s="257"/>
       <c r="B41" s="137" t="s">
         <v>226</v>
       </c>
@@ -7305,7 +7299,7 @@
       <c r="BD41" s="89"/>
     </row>
     <row r="42" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="255"/>
+      <c r="A42" s="257"/>
       <c r="B42" s="136" t="s">
         <v>227</v>
       </c>
@@ -7367,7 +7361,7 @@
       <c r="BD42" s="89"/>
     </row>
     <row r="43" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="255"/>
+      <c r="A43" s="257"/>
       <c r="B43" s="137" t="s">
         <v>228</v>
       </c>
@@ -7431,7 +7425,7 @@
       <c r="BD43" s="89"/>
     </row>
     <row r="44" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="255"/>
+      <c r="A44" s="257"/>
       <c r="B44" s="135"/>
       <c r="C44" s="90" t="s">
         <v>174</v>
@@ -7497,7 +7491,7 @@
       <c r="BD44" s="89"/>
     </row>
     <row r="45" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="255"/>
+      <c r="A45" s="257"/>
       <c r="B45" s="135"/>
       <c r="C45" s="90" t="s">
         <v>173</v>
@@ -7563,7 +7557,7 @@
       <c r="BD45" s="89"/>
     </row>
     <row r="46" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="255"/>
+      <c r="A46" s="257"/>
       <c r="B46" s="136" t="s">
         <v>229</v>
       </c>
@@ -7625,7 +7619,7 @@
       <c r="BD46" s="89"/>
     </row>
     <row r="47" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="255"/>
+      <c r="A47" s="257"/>
       <c r="B47" s="137" t="s">
         <v>230</v>
       </c>
@@ -7693,7 +7687,7 @@
       <c r="BD47" s="89"/>
     </row>
     <row r="48" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="255"/>
+      <c r="A48" s="257"/>
       <c r="B48" s="137" t="s">
         <v>231</v>
       </c>
@@ -7761,7 +7755,7 @@
       <c r="BD48" s="89"/>
     </row>
     <row r="49" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="255"/>
+      <c r="A49" s="257"/>
       <c r="B49" s="137" t="s">
         <v>232</v>
       </c>
@@ -7829,7 +7823,7 @@
       <c r="BD49" s="89"/>
     </row>
     <row r="50" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="255"/>
+      <c r="A50" s="257"/>
       <c r="B50" s="137" t="s">
         <v>233</v>
       </c>
@@ -7897,7 +7891,7 @@
       <c r="BD50" s="89"/>
     </row>
     <row r="51" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="255"/>
+      <c r="A51" s="257"/>
       <c r="B51" s="136" t="s">
         <v>234</v>
       </c>
@@ -7959,7 +7953,7 @@
       <c r="BD51" s="89"/>
     </row>
     <row r="52" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="255"/>
+      <c r="A52" s="257"/>
       <c r="B52" s="137" t="s">
         <v>235</v>
       </c>
@@ -8027,7 +8021,7 @@
       <c r="BD52" s="89"/>
     </row>
     <row r="53" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="255"/>
+      <c r="A53" s="257"/>
       <c r="B53" s="137" t="s">
         <v>236</v>
       </c>
@@ -8095,7 +8089,7 @@
       <c r="BD53" s="89"/>
     </row>
     <row r="54" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="255"/>
+      <c r="A54" s="257"/>
       <c r="B54" s="136" t="s">
         <v>237</v>
       </c>
@@ -8157,7 +8151,7 @@
       <c r="BD54" s="89"/>
     </row>
     <row r="55" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="255"/>
+      <c r="A55" s="257"/>
       <c r="B55" s="137" t="s">
         <v>238</v>
       </c>
@@ -8223,7 +8217,7 @@
       <c r="BD55" s="89"/>
     </row>
     <row r="56" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="255"/>
+      <c r="A56" s="257"/>
       <c r="B56" s="135"/>
       <c r="C56" s="90" t="s">
         <v>183</v>
@@ -8291,7 +8285,7 @@
       <c r="BD56" s="89"/>
     </row>
     <row r="57" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="255"/>
+      <c r="A57" s="257"/>
       <c r="B57" s="135"/>
       <c r="C57" s="90" t="s">
         <v>182</v>
@@ -8359,7 +8353,7 @@
       <c r="BD57" s="89"/>
     </row>
     <row r="58" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="255"/>
+      <c r="A58" s="257"/>
       <c r="B58" s="137" t="s">
         <v>239</v>
       </c>
@@ -8425,7 +8419,7 @@
       <c r="BD58" s="89"/>
     </row>
     <row r="59" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="255"/>
+      <c r="A59" s="257"/>
       <c r="B59" s="135"/>
       <c r="C59" s="90" t="s">
         <v>282</v>
@@ -8493,7 +8487,7 @@
       <c r="BD59" s="89"/>
     </row>
     <row r="60" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="255"/>
+      <c r="A60" s="257"/>
       <c r="B60" s="135"/>
       <c r="C60" s="90" t="s">
         <v>283</v>
@@ -8561,7 +8555,7 @@
       <c r="BD60" s="89"/>
     </row>
     <row r="61" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="255"/>
+      <c r="A61" s="257"/>
       <c r="B61" s="136" t="s">
         <v>240</v>
       </c>
@@ -8623,7 +8617,7 @@
       <c r="BD61" s="89"/>
     </row>
     <row r="62" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="255"/>
+      <c r="A62" s="257"/>
       <c r="B62" s="137" t="s">
         <v>241</v>
       </c>
@@ -8691,7 +8685,7 @@
       <c r="BD62" s="89"/>
     </row>
     <row r="63" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="255"/>
+      <c r="A63" s="257"/>
       <c r="B63" s="137" t="s">
         <v>242</v>
       </c>
@@ -8759,7 +8753,7 @@
       <c r="BD63" s="89"/>
     </row>
     <row r="64" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="255"/>
+      <c r="A64" s="257"/>
       <c r="B64" s="136" t="s">
         <v>243</v>
       </c>
@@ -8821,7 +8815,7 @@
       <c r="BD64" s="89"/>
     </row>
     <row r="65" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="255"/>
+      <c r="A65" s="257"/>
       <c r="B65" s="137" t="s">
         <v>244</v>
       </c>
@@ -8889,7 +8883,7 @@
       <c r="BD65" s="89"/>
     </row>
     <row r="66" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="255"/>
+      <c r="A66" s="257"/>
       <c r="B66" s="136" t="s">
         <v>247</v>
       </c>
@@ -8951,7 +8945,7 @@
       <c r="BD66" s="89"/>
     </row>
     <row r="67" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="255"/>
+      <c r="A67" s="257"/>
       <c r="B67" s="137" t="s">
         <v>248</v>
       </c>
@@ -9019,7 +9013,7 @@
       <c r="BD67" s="89"/>
     </row>
     <row r="68" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="255"/>
+      <c r="A68" s="257"/>
       <c r="B68" s="136" t="s">
         <v>251</v>
       </c>
@@ -9081,7 +9075,7 @@
       <c r="BD68" s="89"/>
     </row>
     <row r="69" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="255"/>
+      <c r="A69" s="257"/>
       <c r="B69" s="137" t="s">
         <v>252</v>
       </c>
@@ -9149,7 +9143,7 @@
       <c r="BD69" s="89"/>
     </row>
     <row r="70" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="255"/>
+      <c r="A70" s="257"/>
       <c r="B70" s="137" t="s">
         <v>253</v>
       </c>
@@ -9217,7 +9211,7 @@
       <c r="BD70" s="89"/>
     </row>
     <row r="71" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="255"/>
+      <c r="A71" s="257"/>
       <c r="B71" s="136" t="s">
         <v>254</v>
       </c>
@@ -9279,7 +9273,7 @@
       <c r="BD71" s="89"/>
     </row>
     <row r="72" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="255"/>
+      <c r="A72" s="257"/>
       <c r="B72" s="137" t="s">
         <v>255</v>
       </c>
@@ -9347,7 +9341,7 @@
       <c r="BD72" s="89"/>
     </row>
     <row r="73" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="255"/>
+      <c r="A73" s="257"/>
       <c r="B73" s="136" t="s">
         <v>256</v>
       </c>
@@ -9409,7 +9403,7 @@
       <c r="BD73" s="89"/>
     </row>
     <row r="74" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="257"/>
+      <c r="A74" s="259"/>
       <c r="B74" s="137" t="s">
         <v>257</v>
       </c>
@@ -9601,7 +9595,7 @@
       <c r="BD76" s="89"/>
     </row>
     <row r="77" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="254" t="s">
+      <c r="A77" s="256" t="s">
         <v>162</v>
       </c>
       <c r="B77" s="135"/>
@@ -9669,7 +9663,7 @@
       <c r="BD77" s="89"/>
     </row>
     <row r="78" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="257"/>
+      <c r="A78" s="259"/>
       <c r="B78" s="135"/>
       <c r="C78" s="90" t="s">
         <v>95</v>
@@ -9797,7 +9791,7 @@
       <c r="BD79" s="89"/>
     </row>
     <row r="80" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="254" t="s">
+      <c r="A80" s="256" t="s">
         <v>162</v>
       </c>
       <c r="B80" s="135"/>
@@ -9865,7 +9859,7 @@
       <c r="BD80" s="89"/>
     </row>
     <row r="81" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="257"/>
+      <c r="A81" s="259"/>
       <c r="B81" s="135"/>
       <c r="C81" s="90" t="s">
         <v>93</v>
@@ -9993,7 +9987,7 @@
       <c r="BD82" s="89"/>
     </row>
     <row r="83" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="254" t="s">
+      <c r="A83" s="256" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="135"/>
@@ -10061,7 +10055,7 @@
       <c r="BD83" s="89"/>
     </row>
     <row r="84" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="257"/>
+      <c r="A84" s="259"/>
       <c r="B84" s="135"/>
       <c r="C84" s="90" t="s">
         <v>134</v>
@@ -10251,7 +10245,7 @@
       <c r="BD86" s="89"/>
     </row>
     <row r="87" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="254" t="s">
+      <c r="A87" s="256" t="s">
         <v>326</v>
       </c>
       <c r="B87" s="135"/>
@@ -10319,7 +10313,7 @@
       <c r="BD87" s="89"/>
     </row>
     <row r="88" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="255"/>
+      <c r="A88" s="257"/>
       <c r="B88" s="135"/>
       <c r="C88" s="95" t="s">
         <v>119</v>
@@ -10385,7 +10379,7 @@
       <c r="BD88" s="89"/>
     </row>
     <row r="89" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="255"/>
+      <c r="A89" s="257"/>
       <c r="B89" s="135"/>
       <c r="C89" s="95" t="s">
         <v>120</v>
@@ -10451,7 +10445,7 @@
       <c r="BD89" s="89"/>
     </row>
     <row r="90" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="255"/>
+      <c r="A90" s="257"/>
       <c r="B90" s="135"/>
       <c r="C90" s="95" t="s">
         <v>121</v>
@@ -10517,7 +10511,7 @@
       <c r="BD90" s="89"/>
     </row>
     <row r="91" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="255"/>
+      <c r="A91" s="257"/>
       <c r="B91" s="135"/>
       <c r="C91" s="95" t="s">
         <v>122</v>
@@ -10583,7 +10577,7 @@
       <c r="BD91" s="89"/>
     </row>
     <row r="92" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="255"/>
+      <c r="A92" s="257"/>
       <c r="B92" s="135"/>
       <c r="C92" s="95" t="s">
         <v>123</v>
@@ -10649,7 +10643,7 @@
       <c r="BD92" s="89"/>
     </row>
     <row r="93" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="255"/>
+      <c r="A93" s="257"/>
       <c r="B93" s="135"/>
       <c r="C93" s="95" t="s">
         <v>124</v>
@@ -10715,7 +10709,7 @@
       <c r="BD93" s="89"/>
     </row>
     <row r="94" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="255"/>
+      <c r="A94" s="257"/>
       <c r="B94" s="135"/>
       <c r="C94" s="95" t="s">
         <v>125</v>
@@ -10781,7 +10775,7 @@
       <c r="BD94" s="89"/>
     </row>
     <row r="95" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="255"/>
+      <c r="A95" s="257"/>
       <c r="B95" s="135"/>
       <c r="C95" s="95" t="s">
         <v>126</v>
@@ -10847,7 +10841,7 @@
       <c r="BD95" s="89"/>
     </row>
     <row r="96" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="255"/>
+      <c r="A96" s="257"/>
       <c r="B96" s="135"/>
       <c r="C96" s="95" t="s">
         <v>127</v>
@@ -10913,7 +10907,7 @@
       <c r="BD96" s="89"/>
     </row>
     <row r="97" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="255"/>
+      <c r="A97" s="257"/>
       <c r="B97" s="135"/>
       <c r="C97" s="95" t="s">
         <v>128</v>
@@ -10979,7 +10973,7 @@
       <c r="BD97" s="89"/>
     </row>
     <row r="98" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="255"/>
+      <c r="A98" s="257"/>
       <c r="B98" s="135"/>
       <c r="C98" s="95" t="s">
         <v>129</v>
@@ -11045,7 +11039,7 @@
       <c r="BD98" s="89"/>
     </row>
     <row r="99" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="255"/>
+      <c r="A99" s="257"/>
       <c r="B99" s="135"/>
       <c r="C99" s="95" t="s">
         <v>130</v>
@@ -11111,7 +11105,7 @@
       <c r="BD99" s="89"/>
     </row>
     <row r="100" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="255"/>
+      <c r="A100" s="257"/>
       <c r="B100" s="135"/>
       <c r="C100" s="95" t="s">
         <v>131</v>
@@ -11177,7 +11171,7 @@
       <c r="BD100" s="89"/>
     </row>
     <row r="101" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="255"/>
+      <c r="A101" s="257"/>
       <c r="B101" s="135"/>
       <c r="C101" s="95" t="s">
         <v>132</v>
@@ -11243,7 +11237,7 @@
       <c r="BD101" s="89"/>
     </row>
     <row r="102" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="257"/>
+      <c r="A102" s="259"/>
       <c r="B102" s="135"/>
       <c r="C102" s="95" t="s">
         <v>133</v>
@@ -11371,7 +11365,7 @@
       <c r="BD103" s="89"/>
     </row>
     <row r="104" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="254" t="s">
+      <c r="A104" s="256" t="s">
         <v>325</v>
       </c>
       <c r="B104" s="136" t="s">
@@ -11435,7 +11429,7 @@
       <c r="BD104" s="89"/>
     </row>
     <row r="105" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="255"/>
+      <c r="A105" s="257"/>
       <c r="B105" s="137">
         <v>3.0101010000000001</v>
       </c>
@@ -11503,7 +11497,7 @@
       <c r="BD105" s="89"/>
     </row>
     <row r="106" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="255"/>
+      <c r="A106" s="257"/>
       <c r="B106" s="136" t="s">
         <v>224</v>
       </c>
@@ -11565,7 +11559,7 @@
       <c r="BD106" s="89"/>
     </row>
     <row r="107" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="255"/>
+      <c r="A107" s="257"/>
       <c r="B107" s="137" t="s">
         <v>164</v>
       </c>
@@ -11633,7 +11627,7 @@
       <c r="BD107" s="89"/>
     </row>
     <row r="108" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="255"/>
+      <c r="A108" s="257"/>
       <c r="B108" s="137" t="s">
         <v>165</v>
       </c>
@@ -11701,7 +11695,7 @@
       <c r="BD108" s="89"/>
     </row>
     <row r="109" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="255"/>
+      <c r="A109" s="257"/>
       <c r="B109" s="136" t="s">
         <v>225</v>
       </c>
@@ -11763,7 +11757,7 @@
       <c r="BD109" s="89"/>
     </row>
     <row r="110" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="255"/>
+      <c r="A110" s="257"/>
       <c r="B110" s="137" t="s">
         <v>226</v>
       </c>
@@ -11831,7 +11825,7 @@
       <c r="BD110" s="89"/>
     </row>
     <row r="111" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="255"/>
+      <c r="A111" s="257"/>
       <c r="B111" s="136" t="s">
         <v>227</v>
       </c>
@@ -11893,7 +11887,7 @@
       <c r="BD111" s="89"/>
     </row>
     <row r="112" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="255"/>
+      <c r="A112" s="257"/>
       <c r="B112" s="137" t="s">
         <v>228</v>
       </c>
@@ -11961,7 +11955,7 @@
       <c r="BD112" s="89"/>
     </row>
     <row r="113" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="255"/>
+      <c r="A113" s="257"/>
       <c r="B113" s="135"/>
       <c r="C113" s="90" t="s">
         <v>174</v>
@@ -12027,7 +12021,7 @@
       <c r="BD113" s="89"/>
     </row>
     <row r="114" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="255"/>
+      <c r="A114" s="257"/>
       <c r="B114" s="135"/>
       <c r="C114" s="90" t="s">
         <v>173</v>
@@ -12093,7 +12087,7 @@
       <c r="BD114" s="89"/>
     </row>
     <row r="115" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="255"/>
+      <c r="A115" s="257"/>
       <c r="B115" s="136" t="s">
         <v>229</v>
       </c>
@@ -12155,7 +12149,7 @@
       <c r="BD115" s="89"/>
     </row>
     <row r="116" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="255"/>
+      <c r="A116" s="257"/>
       <c r="B116" s="137" t="s">
         <v>230</v>
       </c>
@@ -12223,7 +12217,7 @@
       <c r="BD116" s="89"/>
     </row>
     <row r="117" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="255"/>
+      <c r="A117" s="257"/>
       <c r="B117" s="137" t="s">
         <v>231</v>
       </c>
@@ -12291,7 +12285,7 @@
       <c r="BD117" s="89"/>
     </row>
     <row r="118" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="255"/>
+      <c r="A118" s="257"/>
       <c r="B118" s="137" t="s">
         <v>232</v>
       </c>
@@ -12359,7 +12353,7 @@
       <c r="BD118" s="89"/>
     </row>
     <row r="119" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="255"/>
+      <c r="A119" s="257"/>
       <c r="B119" s="137" t="s">
         <v>233</v>
       </c>
@@ -12427,7 +12421,7 @@
       <c r="BD119" s="89"/>
     </row>
     <row r="120" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="255"/>
+      <c r="A120" s="257"/>
       <c r="B120" s="136" t="s">
         <v>234</v>
       </c>
@@ -12489,7 +12483,7 @@
       <c r="BD120" s="89"/>
     </row>
     <row r="121" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="255"/>
+      <c r="A121" s="257"/>
       <c r="B121" s="137" t="s">
         <v>235</v>
       </c>
@@ -12557,7 +12551,7 @@
       <c r="BD121" s="89"/>
     </row>
     <row r="122" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="255"/>
+      <c r="A122" s="257"/>
       <c r="B122" s="137" t="s">
         <v>236</v>
       </c>
@@ -12625,7 +12619,7 @@
       <c r="BD122" s="89"/>
     </row>
     <row r="123" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="255"/>
+      <c r="A123" s="257"/>
       <c r="B123" s="136" t="s">
         <v>237</v>
       </c>
@@ -12687,7 +12681,7 @@
       <c r="BD123" s="89"/>
     </row>
     <row r="124" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="255"/>
+      <c r="A124" s="257"/>
       <c r="B124" s="137" t="s">
         <v>238</v>
       </c>
@@ -12751,7 +12745,7 @@
       <c r="BD124" s="89"/>
     </row>
     <row r="125" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="255"/>
+      <c r="A125" s="257"/>
       <c r="B125" s="135"/>
       <c r="C125" s="90" t="s">
         <v>183</v>
@@ -12817,7 +12811,7 @@
       <c r="BD125" s="89"/>
     </row>
     <row r="126" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="255"/>
+      <c r="A126" s="257"/>
       <c r="B126" s="135"/>
       <c r="C126" s="90" t="s">
         <v>182</v>
@@ -12883,7 +12877,7 @@
       <c r="BD126" s="89"/>
     </row>
     <row r="127" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="255"/>
+      <c r="A127" s="257"/>
       <c r="B127" s="137" t="s">
         <v>239</v>
       </c>
@@ -12947,7 +12941,7 @@
       <c r="BD127" s="89"/>
     </row>
     <row r="128" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="255"/>
+      <c r="A128" s="257"/>
       <c r="B128" s="135"/>
       <c r="C128" s="90" t="s">
         <v>282</v>
@@ -13013,7 +13007,7 @@
       <c r="BD128" s="89"/>
     </row>
     <row r="129" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="255"/>
+      <c r="A129" s="257"/>
       <c r="B129" s="135"/>
       <c r="C129" s="90" t="s">
         <v>283</v>
@@ -13079,7 +13073,7 @@
       <c r="BD129" s="89"/>
     </row>
     <row r="130" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="255"/>
+      <c r="A130" s="257"/>
       <c r="B130" s="136" t="s">
         <v>240</v>
       </c>
@@ -13141,7 +13135,7 @@
       <c r="BD130" s="89"/>
     </row>
     <row r="131" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="255"/>
+      <c r="A131" s="257"/>
       <c r="B131" s="137" t="s">
         <v>241</v>
       </c>
@@ -13209,7 +13203,7 @@
       <c r="BD131" s="89"/>
     </row>
     <row r="132" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="255"/>
+      <c r="A132" s="257"/>
       <c r="B132" s="137" t="s">
         <v>242</v>
       </c>
@@ -13277,7 +13271,7 @@
       <c r="BD132" s="89"/>
     </row>
     <row r="133" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="255"/>
+      <c r="A133" s="257"/>
       <c r="B133" s="136" t="s">
         <v>243</v>
       </c>
@@ -13339,7 +13333,7 @@
       <c r="BD133" s="89"/>
     </row>
     <row r="134" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="255"/>
+      <c r="A134" s="257"/>
       <c r="B134" s="137" t="s">
         <v>244</v>
       </c>
@@ -13407,7 +13401,7 @@
       <c r="BD134" s="89"/>
     </row>
     <row r="135" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="255"/>
+      <c r="A135" s="257"/>
       <c r="B135" s="136" t="s">
         <v>247</v>
       </c>
@@ -13469,7 +13463,7 @@
       <c r="BD135" s="89"/>
     </row>
     <row r="136" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="255"/>
+      <c r="A136" s="257"/>
       <c r="B136" s="137" t="s">
         <v>248</v>
       </c>
@@ -13537,7 +13531,7 @@
       <c r="BD136" s="89"/>
     </row>
     <row r="137" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="255"/>
+      <c r="A137" s="257"/>
       <c r="B137" s="136" t="s">
         <v>249</v>
       </c>
@@ -13599,7 +13593,7 @@
       <c r="BD137" s="89"/>
     </row>
     <row r="138" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="255"/>
+      <c r="A138" s="257"/>
       <c r="B138" s="137" t="s">
         <v>250</v>
       </c>
@@ -13667,7 +13661,7 @@
       <c r="BD138" s="89"/>
     </row>
     <row r="139" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="255"/>
+      <c r="A139" s="257"/>
       <c r="B139" s="136" t="s">
         <v>251</v>
       </c>
@@ -13729,7 +13723,7 @@
       <c r="BD139" s="89"/>
     </row>
     <row r="140" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="255"/>
+      <c r="A140" s="257"/>
       <c r="B140" s="137" t="s">
         <v>252</v>
       </c>
@@ -13797,7 +13791,7 @@
       <c r="BD140" s="89"/>
     </row>
     <row r="141" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="255"/>
+      <c r="A141" s="257"/>
       <c r="B141" s="137" t="s">
         <v>253</v>
       </c>
@@ -13865,7 +13859,7 @@
       <c r="BD141" s="89"/>
     </row>
     <row r="142" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="255"/>
+      <c r="A142" s="257"/>
       <c r="B142" s="136" t="s">
         <v>254</v>
       </c>
@@ -13927,7 +13921,7 @@
       <c r="BD142" s="89"/>
     </row>
     <row r="143" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="255"/>
+      <c r="A143" s="257"/>
       <c r="B143" s="137" t="s">
         <v>255</v>
       </c>
@@ -13995,7 +13989,7 @@
       <c r="BD143" s="89"/>
     </row>
     <row r="144" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="255"/>
+      <c r="A144" s="257"/>
       <c r="B144" s="136" t="s">
         <v>256</v>
       </c>
@@ -14057,7 +14051,7 @@
       <c r="BD144" s="89"/>
     </row>
     <row r="145" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="255"/>
+      <c r="A145" s="257"/>
       <c r="B145" s="137" t="s">
         <v>257</v>
       </c>
@@ -14125,7 +14119,7 @@
       <c r="BD145" s="89"/>
     </row>
     <row r="146" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="255"/>
+      <c r="A146" s="257"/>
       <c r="B146" s="136" t="s">
         <v>258</v>
       </c>
@@ -14187,7 +14181,7 @@
       <c r="BD146" s="89"/>
     </row>
     <row r="147" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="255"/>
+      <c r="A147" s="257"/>
       <c r="B147" s="137" t="s">
         <v>259</v>
       </c>
@@ -14255,7 +14249,7 @@
       <c r="BD147" s="89"/>
     </row>
     <row r="148" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="255"/>
+      <c r="A148" s="257"/>
       <c r="B148" s="136" t="s">
         <v>260</v>
       </c>
@@ -14317,7 +14311,7 @@
       <c r="BD148" s="89"/>
     </row>
     <row r="149" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="255"/>
+      <c r="A149" s="257"/>
       <c r="B149" s="137" t="s">
         <v>261</v>
       </c>
@@ -14385,7 +14379,7 @@
       <c r="BD149" s="89"/>
     </row>
     <row r="150" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="255"/>
+      <c r="A150" s="257"/>
       <c r="B150" s="137" t="s">
         <v>262</v>
       </c>
@@ -14453,7 +14447,7 @@
       <c r="BD150" s="89"/>
     </row>
     <row r="151" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="255"/>
+      <c r="A151" s="257"/>
       <c r="B151" s="137" t="s">
         <v>263</v>
       </c>
@@ -14521,7 +14515,7 @@
       <c r="BD151" s="89"/>
     </row>
     <row r="152" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="255"/>
+      <c r="A152" s="257"/>
       <c r="B152" s="137" t="s">
         <v>264</v>
       </c>
@@ -14589,7 +14583,7 @@
       <c r="BD152" s="89"/>
     </row>
     <row r="153" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="255"/>
+      <c r="A153" s="257"/>
       <c r="B153" s="136" t="s">
         <v>265</v>
       </c>
@@ -14651,7 +14645,7 @@
       <c r="BD153" s="89"/>
     </row>
     <row r="154" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="255"/>
+      <c r="A154" s="257"/>
       <c r="B154" s="137" t="s">
         <v>266</v>
       </c>
@@ -14719,7 +14713,7 @@
       <c r="BD154" s="89"/>
     </row>
     <row r="155" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="255"/>
+      <c r="A155" s="257"/>
       <c r="B155" s="137" t="s">
         <v>267</v>
       </c>
@@ -14787,7 +14781,7 @@
       <c r="BD155" s="89"/>
     </row>
     <row r="156" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="255"/>
+      <c r="A156" s="257"/>
       <c r="B156" s="136" t="s">
         <v>268</v>
       </c>
@@ -14849,7 +14843,7 @@
       <c r="BD156" s="89"/>
     </row>
     <row r="157" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="255"/>
+      <c r="A157" s="257"/>
       <c r="B157" s="137" t="s">
         <v>269</v>
       </c>
@@ -14917,7 +14911,7 @@
       <c r="BD157" s="89"/>
     </row>
     <row r="158" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="255"/>
+      <c r="A158" s="257"/>
       <c r="B158" s="137" t="s">
         <v>270</v>
       </c>
@@ -14985,7 +14979,7 @@
       <c r="BD158" s="89"/>
     </row>
     <row r="159" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="255"/>
+      <c r="A159" s="257"/>
       <c r="B159" s="137" t="s">
         <v>271</v>
       </c>
@@ -15053,7 +15047,7 @@
       <c r="BD159" s="89"/>
     </row>
     <row r="160" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="255"/>
+      <c r="A160" s="257"/>
       <c r="B160" s="137" t="s">
         <v>272</v>
       </c>
@@ -15121,7 +15115,7 @@
       <c r="BD160" s="89"/>
     </row>
     <row r="161" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="255"/>
+      <c r="A161" s="257"/>
       <c r="B161" s="136" t="s">
         <v>273</v>
       </c>
@@ -15183,7 +15177,7 @@
       <c r="BD161" s="89"/>
     </row>
     <row r="162" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="255"/>
+      <c r="A162" s="257"/>
       <c r="B162" s="137" t="s">
         <v>274</v>
       </c>
@@ -15251,7 +15245,7 @@
       <c r="BD162" s="89"/>
     </row>
     <row r="163" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="255"/>
+      <c r="A163" s="257"/>
       <c r="B163" s="137" t="s">
         <v>275</v>
       </c>
@@ -15319,7 +15313,7 @@
       <c r="BD163" s="89"/>
     </row>
     <row r="164" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="255"/>
+      <c r="A164" s="257"/>
       <c r="B164" s="136" t="s">
         <v>276</v>
       </c>
@@ -15381,7 +15375,7 @@
       <c r="BD164" s="89"/>
     </row>
     <row r="165" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="255"/>
+      <c r="A165" s="257"/>
       <c r="B165" s="137" t="s">
         <v>277</v>
       </c>
@@ -15449,7 +15443,7 @@
       <c r="BD165" s="89"/>
     </row>
     <row r="166" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="255"/>
+      <c r="A166" s="257"/>
       <c r="B166" s="137" t="s">
         <v>278</v>
       </c>
@@ -15517,7 +15511,7 @@
       <c r="BD166" s="89"/>
     </row>
     <row r="167" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="255"/>
+      <c r="A167" s="257"/>
       <c r="B167" s="136" t="s">
         <v>279</v>
       </c>
@@ -15579,7 +15573,7 @@
       <c r="BD167" s="89"/>
     </row>
     <row r="168" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="256"/>
+      <c r="A168" s="258"/>
       <c r="B168" s="138" t="s">
         <v>280</v>
       </c>
@@ -15719,74 +15713,74 @@
         <f>SUM(K170:BD170)</f>
         <v>3500</v>
       </c>
-      <c r="E170" s="239" t="s">
+      <c r="E170" s="241" t="s">
         <v>331</v>
       </c>
-      <c r="F170" s="239"/>
-      <c r="G170" s="239"/>
-      <c r="H170" s="234"/>
-      <c r="I170" s="232"/>
-      <c r="J170" s="232"/>
-      <c r="K170" s="232">
+      <c r="F170" s="241"/>
+      <c r="G170" s="241"/>
+      <c r="H170" s="236"/>
+      <c r="I170" s="234"/>
+      <c r="J170" s="234"/>
+      <c r="K170" s="234">
         <v>500</v>
       </c>
-      <c r="L170" s="232"/>
-      <c r="M170" s="232"/>
-      <c r="N170" s="233"/>
-      <c r="O170" s="234"/>
-      <c r="P170" s="232"/>
-      <c r="Q170" s="232"/>
-      <c r="R170" s="232">
+      <c r="L170" s="234"/>
+      <c r="M170" s="234"/>
+      <c r="N170" s="235"/>
+      <c r="O170" s="236"/>
+      <c r="P170" s="234"/>
+      <c r="Q170" s="234"/>
+      <c r="R170" s="234">
         <v>500</v>
       </c>
-      <c r="S170" s="232"/>
-      <c r="T170" s="232"/>
-      <c r="U170" s="233"/>
-      <c r="V170" s="234"/>
-      <c r="W170" s="232"/>
-      <c r="X170" s="232"/>
-      <c r="Y170" s="232">
+      <c r="S170" s="234"/>
+      <c r="T170" s="234"/>
+      <c r="U170" s="235"/>
+      <c r="V170" s="236"/>
+      <c r="W170" s="234"/>
+      <c r="X170" s="234"/>
+      <c r="Y170" s="234">
         <v>500</v>
       </c>
-      <c r="Z170" s="232"/>
-      <c r="AA170" s="232"/>
-      <c r="AB170" s="233"/>
-      <c r="AC170" s="234"/>
-      <c r="AD170" s="232"/>
-      <c r="AE170" s="232"/>
-      <c r="AF170" s="232">
+      <c r="Z170" s="234"/>
+      <c r="AA170" s="234"/>
+      <c r="AB170" s="235"/>
+      <c r="AC170" s="236"/>
+      <c r="AD170" s="234"/>
+      <c r="AE170" s="234"/>
+      <c r="AF170" s="234">
         <v>500</v>
       </c>
-      <c r="AG170" s="232"/>
-      <c r="AH170" s="232"/>
-      <c r="AI170" s="233"/>
-      <c r="AJ170" s="234"/>
-      <c r="AK170" s="232"/>
-      <c r="AL170" s="232"/>
-      <c r="AM170" s="232">
+      <c r="AG170" s="234"/>
+      <c r="AH170" s="234"/>
+      <c r="AI170" s="235"/>
+      <c r="AJ170" s="236"/>
+      <c r="AK170" s="234"/>
+      <c r="AL170" s="234"/>
+      <c r="AM170" s="234">
         <v>500</v>
       </c>
-      <c r="AN170" s="232"/>
-      <c r="AO170" s="232"/>
-      <c r="AP170" s="233"/>
-      <c r="AQ170" s="234"/>
-      <c r="AR170" s="232"/>
-      <c r="AS170" s="232"/>
-      <c r="AT170" s="232">
+      <c r="AN170" s="234"/>
+      <c r="AO170" s="234"/>
+      <c r="AP170" s="235"/>
+      <c r="AQ170" s="236"/>
+      <c r="AR170" s="234"/>
+      <c r="AS170" s="234"/>
+      <c r="AT170" s="234">
         <v>500</v>
       </c>
-      <c r="AU170" s="232"/>
-      <c r="AV170" s="232"/>
-      <c r="AW170" s="233"/>
-      <c r="AX170" s="234"/>
-      <c r="AY170" s="232"/>
-      <c r="AZ170" s="232"/>
-      <c r="BA170" s="232">
+      <c r="AU170" s="234"/>
+      <c r="AV170" s="234"/>
+      <c r="AW170" s="235"/>
+      <c r="AX170" s="236"/>
+      <c r="AY170" s="234"/>
+      <c r="AZ170" s="234"/>
+      <c r="BA170" s="234">
         <v>500</v>
       </c>
-      <c r="BB170" s="232"/>
-      <c r="BC170" s="232"/>
-      <c r="BD170" s="233"/>
+      <c r="BB170" s="234"/>
+      <c r="BC170" s="234"/>
+      <c r="BD170" s="235"/>
     </row>
     <row r="171" spans="1:56" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A171" s="150"/>
@@ -15798,74 +15792,74 @@
         <f>SUM(K171:BD171)</f>
         <v>4410</v>
       </c>
-      <c r="E171" s="239" t="s">
+      <c r="E171" s="241" t="s">
         <v>330</v>
       </c>
-      <c r="F171" s="239"/>
-      <c r="G171" s="239"/>
-      <c r="H171" s="234"/>
-      <c r="I171" s="232"/>
-      <c r="J171" s="232"/>
-      <c r="K171" s="232">
+      <c r="F171" s="241"/>
+      <c r="G171" s="241"/>
+      <c r="H171" s="236"/>
+      <c r="I171" s="234"/>
+      <c r="J171" s="234"/>
+      <c r="K171" s="234">
         <v>630</v>
       </c>
-      <c r="L171" s="232"/>
-      <c r="M171" s="232"/>
-      <c r="N171" s="233"/>
-      <c r="O171" s="234"/>
-      <c r="P171" s="232"/>
-      <c r="Q171" s="232"/>
-      <c r="R171" s="232">
+      <c r="L171" s="234"/>
+      <c r="M171" s="234"/>
+      <c r="N171" s="235"/>
+      <c r="O171" s="236"/>
+      <c r="P171" s="234"/>
+      <c r="Q171" s="234"/>
+      <c r="R171" s="234">
         <v>630</v>
       </c>
-      <c r="S171" s="232"/>
-      <c r="T171" s="232"/>
-      <c r="U171" s="233"/>
-      <c r="V171" s="234"/>
-      <c r="W171" s="232"/>
-      <c r="X171" s="232"/>
-      <c r="Y171" s="232">
+      <c r="S171" s="234"/>
+      <c r="T171" s="234"/>
+      <c r="U171" s="235"/>
+      <c r="V171" s="236"/>
+      <c r="W171" s="234"/>
+      <c r="X171" s="234"/>
+      <c r="Y171" s="234">
         <v>630</v>
       </c>
-      <c r="Z171" s="232"/>
-      <c r="AA171" s="232"/>
-      <c r="AB171" s="233"/>
-      <c r="AC171" s="234"/>
-      <c r="AD171" s="232"/>
-      <c r="AE171" s="232"/>
-      <c r="AF171" s="232">
+      <c r="Z171" s="234"/>
+      <c r="AA171" s="234"/>
+      <c r="AB171" s="235"/>
+      <c r="AC171" s="236"/>
+      <c r="AD171" s="234"/>
+      <c r="AE171" s="234"/>
+      <c r="AF171" s="234">
         <v>630</v>
       </c>
-      <c r="AG171" s="232"/>
-      <c r="AH171" s="232"/>
-      <c r="AI171" s="233"/>
-      <c r="AJ171" s="234"/>
-      <c r="AK171" s="232"/>
-      <c r="AL171" s="232"/>
-      <c r="AM171" s="232">
+      <c r="AG171" s="234"/>
+      <c r="AH171" s="234"/>
+      <c r="AI171" s="235"/>
+      <c r="AJ171" s="236"/>
+      <c r="AK171" s="234"/>
+      <c r="AL171" s="234"/>
+      <c r="AM171" s="234">
         <v>630</v>
       </c>
-      <c r="AN171" s="232"/>
-      <c r="AO171" s="232"/>
-      <c r="AP171" s="233"/>
-      <c r="AQ171" s="234"/>
-      <c r="AR171" s="232"/>
-      <c r="AS171" s="232"/>
-      <c r="AT171" s="232">
+      <c r="AN171" s="234"/>
+      <c r="AO171" s="234"/>
+      <c r="AP171" s="235"/>
+      <c r="AQ171" s="236"/>
+      <c r="AR171" s="234"/>
+      <c r="AS171" s="234"/>
+      <c r="AT171" s="234">
         <v>630</v>
       </c>
-      <c r="AU171" s="232"/>
-      <c r="AV171" s="232"/>
-      <c r="AW171" s="233"/>
-      <c r="AX171" s="234"/>
-      <c r="AY171" s="232"/>
-      <c r="AZ171" s="232"/>
-      <c r="BA171" s="232">
+      <c r="AU171" s="234"/>
+      <c r="AV171" s="234"/>
+      <c r="AW171" s="235"/>
+      <c r="AX171" s="236"/>
+      <c r="AY171" s="234"/>
+      <c r="AZ171" s="234"/>
+      <c r="BA171" s="234">
         <v>630</v>
       </c>
-      <c r="BB171" s="232"/>
-      <c r="BC171" s="232"/>
-      <c r="BD171" s="233"/>
+      <c r="BB171" s="234"/>
+      <c r="BC171" s="234"/>
+      <c r="BD171" s="235"/>
     </row>
     <row r="172" spans="1:56" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="152"/>
@@ -15877,74 +15871,74 @@
         <f>+D169+D171</f>
         <v>9910</v>
       </c>
-      <c r="E172" s="248" t="s">
+      <c r="E172" s="250" t="s">
         <v>314</v>
       </c>
-      <c r="F172" s="248"/>
-      <c r="G172" s="248"/>
-      <c r="H172" s="250"/>
-      <c r="I172" s="251"/>
-      <c r="J172" s="251"/>
-      <c r="K172" s="252">
+      <c r="F172" s="250"/>
+      <c r="G172" s="250"/>
+      <c r="H172" s="252"/>
+      <c r="I172" s="253"/>
+      <c r="J172" s="253"/>
+      <c r="K172" s="254">
         <v>44607</v>
       </c>
-      <c r="L172" s="252"/>
-      <c r="M172" s="252"/>
-      <c r="N172" s="253"/>
-      <c r="O172" s="250"/>
-      <c r="P172" s="251"/>
-      <c r="Q172" s="251"/>
-      <c r="R172" s="252">
+      <c r="L172" s="254"/>
+      <c r="M172" s="254"/>
+      <c r="N172" s="255"/>
+      <c r="O172" s="252"/>
+      <c r="P172" s="253"/>
+      <c r="Q172" s="253"/>
+      <c r="R172" s="254">
         <v>44607</v>
       </c>
-      <c r="S172" s="252"/>
-      <c r="T172" s="252"/>
-      <c r="U172" s="253"/>
-      <c r="V172" s="250"/>
-      <c r="W172" s="251"/>
-      <c r="X172" s="251"/>
-      <c r="Y172" s="252">
+      <c r="S172" s="254"/>
+      <c r="T172" s="254"/>
+      <c r="U172" s="255"/>
+      <c r="V172" s="252"/>
+      <c r="W172" s="253"/>
+      <c r="X172" s="253"/>
+      <c r="Y172" s="254">
         <v>44607</v>
       </c>
-      <c r="Z172" s="252"/>
-      <c r="AA172" s="252"/>
-      <c r="AB172" s="253"/>
-      <c r="AC172" s="250"/>
-      <c r="AD172" s="251"/>
-      <c r="AE172" s="251"/>
-      <c r="AF172" s="252">
+      <c r="Z172" s="254"/>
+      <c r="AA172" s="254"/>
+      <c r="AB172" s="255"/>
+      <c r="AC172" s="252"/>
+      <c r="AD172" s="253"/>
+      <c r="AE172" s="253"/>
+      <c r="AF172" s="254">
         <v>44607</v>
       </c>
-      <c r="AG172" s="252"/>
-      <c r="AH172" s="252"/>
-      <c r="AI172" s="253"/>
-      <c r="AJ172" s="250"/>
-      <c r="AK172" s="251"/>
-      <c r="AL172" s="251"/>
-      <c r="AM172" s="252">
+      <c r="AG172" s="254"/>
+      <c r="AH172" s="254"/>
+      <c r="AI172" s="255"/>
+      <c r="AJ172" s="252"/>
+      <c r="AK172" s="253"/>
+      <c r="AL172" s="253"/>
+      <c r="AM172" s="254">
         <v>44607</v>
       </c>
-      <c r="AN172" s="252"/>
-      <c r="AO172" s="252"/>
-      <c r="AP172" s="253"/>
-      <c r="AQ172" s="250"/>
-      <c r="AR172" s="251"/>
-      <c r="AS172" s="251"/>
-      <c r="AT172" s="252">
+      <c r="AN172" s="254"/>
+      <c r="AO172" s="254"/>
+      <c r="AP172" s="255"/>
+      <c r="AQ172" s="252"/>
+      <c r="AR172" s="253"/>
+      <c r="AS172" s="253"/>
+      <c r="AT172" s="254">
         <v>44607</v>
       </c>
-      <c r="AU172" s="252"/>
-      <c r="AV172" s="252"/>
-      <c r="AW172" s="253"/>
-      <c r="AX172" s="250"/>
-      <c r="AY172" s="251"/>
-      <c r="AZ172" s="251"/>
-      <c r="BA172" s="252">
+      <c r="AU172" s="254"/>
+      <c r="AV172" s="254"/>
+      <c r="AW172" s="255"/>
+      <c r="AX172" s="252"/>
+      <c r="AY172" s="253"/>
+      <c r="AZ172" s="253"/>
+      <c r="BA172" s="254">
         <v>44607</v>
       </c>
-      <c r="BB172" s="252"/>
-      <c r="BC172" s="252"/>
-      <c r="BD172" s="253"/>
+      <c r="BB172" s="254"/>
+      <c r="BC172" s="254"/>
+      <c r="BD172" s="255"/>
     </row>
     <row r="173" spans="1:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="163"/>
@@ -16173,10 +16167,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD19"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="G1" zoomScale="119" zoomScaleNormal="172" zoomScaleSheetLayoutView="172" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="134" zoomScaleNormal="134" zoomScaleSheetLayoutView="119" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3:Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -16196,7 +16190,7 @@
     <col min="30" max="16384" width="11.42578125" style="180"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="291" t="s">
         <v>381</v>
       </c>
@@ -16210,28 +16204,26 @@
       <c r="I1" s="292"/>
       <c r="J1" s="292"/>
       <c r="K1" s="292"/>
-      <c r="L1" s="302" t="s">
+      <c r="L1" s="332" t="s">
         <v>382</v>
       </c>
-      <c r="M1" s="302"/>
-      <c r="N1" s="302"/>
-      <c r="O1" s="302"/>
-      <c r="P1" s="302"/>
-      <c r="Q1" s="302"/>
-      <c r="R1" s="302"/>
-      <c r="S1" s="302"/>
-      <c r="T1" s="292" t="s">
-        <v>383</v>
-      </c>
-      <c r="U1" s="292"/>
-      <c r="V1" s="292"/>
-      <c r="W1" s="292"/>
-      <c r="X1" s="292"/>
-      <c r="Y1" s="292"/>
-      <c r="Z1" s="292"/>
+      <c r="M1" s="332"/>
+      <c r="N1" s="332"/>
+      <c r="O1" s="332"/>
+      <c r="P1" s="332"/>
+      <c r="Q1" s="332"/>
+      <c r="R1" s="332"/>
+      <c r="S1" s="332"/>
+      <c r="T1" s="332"/>
+      <c r="U1" s="332"/>
+      <c r="V1" s="332"/>
+      <c r="W1" s="332"/>
+      <c r="X1" s="332"/>
+      <c r="Y1" s="332"/>
+      <c r="Z1" s="332"/>
       <c r="AA1" s="199"/>
     </row>
-    <row r="2" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="187" t="s">
         <v>294</v>
       </c>
@@ -16246,7 +16238,7 @@
       </c>
       <c r="G2" s="286"/>
       <c r="H2" s="289" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I2" s="289"/>
       <c r="J2" s="289"/>
@@ -16270,7 +16262,7 @@
       <c r="AB2" s="289"/>
       <c r="AC2" s="290"/>
     </row>
-    <row r="3" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="187" t="s">
         <v>362</v>
       </c>
@@ -16284,20 +16276,20 @@
         <v>338</v>
       </c>
       <c r="G3" s="286"/>
-      <c r="H3" s="312">
+      <c r="H3" s="311">
         <v>71252646</v>
       </c>
-      <c r="I3" s="312"/>
-      <c r="J3" s="313" t="s">
+      <c r="I3" s="311"/>
+      <c r="J3" s="312" t="s">
         <v>342</v>
       </c>
-      <c r="K3" s="313"/>
-      <c r="L3" s="313"/>
-      <c r="M3" s="313"/>
-      <c r="N3" s="311" t="s">
+      <c r="K3" s="312"/>
+      <c r="L3" s="312"/>
+      <c r="M3" s="312"/>
+      <c r="N3" s="310" t="s">
         <v>379</v>
       </c>
-      <c r="O3" s="311"/>
+      <c r="O3" s="310"/>
       <c r="P3" s="300" t="s">
         <v>312</v>
       </c>
@@ -16308,16 +16300,16 @@
       <c r="U3" s="300"/>
       <c r="V3" s="300"/>
       <c r="W3" s="300"/>
-      <c r="X3" s="303">
+      <c r="X3" s="302">
         <f>ROUND(+F13*0.3,0)</f>
         <v>0</v>
       </c>
-      <c r="Y3" s="303"/>
+      <c r="Y3" s="302"/>
       <c r="Z3" s="184"/>
       <c r="AA3" s="184"/>
       <c r="AB3" s="183"/>
     </row>
-    <row r="4" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="187" t="s">
         <v>363</v>
       </c>
@@ -16333,12 +16325,12 @@
         <v>973439458</v>
       </c>
       <c r="I4" s="284"/>
-      <c r="J4" s="310" t="s">
+      <c r="J4" s="309" t="s">
         <v>343</v>
       </c>
-      <c r="K4" s="310"/>
-      <c r="L4" s="310"/>
-      <c r="M4" s="310"/>
+      <c r="K4" s="309"/>
+      <c r="L4" s="309"/>
+      <c r="M4" s="309"/>
       <c r="N4" s="284">
         <v>103</v>
       </c>
@@ -16353,15 +16345,15 @@
       <c r="U4" s="301"/>
       <c r="V4" s="301"/>
       <c r="W4" s="301"/>
-      <c r="X4" s="304">
+      <c r="X4" s="303">
         <f>18*1000/30</f>
         <v>600</v>
       </c>
-      <c r="Y4" s="304"/>
+      <c r="Y4" s="303"/>
       <c r="Z4" s="185"/>
       <c r="AA4" s="185"/>
     </row>
-    <row r="5" spans="1:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="188" t="s">
         <v>309</v>
       </c>
@@ -16376,7 +16368,7 @@
       </c>
       <c r="G5" s="296"/>
       <c r="H5" s="284" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I5" s="284"/>
       <c r="J5" s="284"/>
@@ -16386,73 +16378,70 @@
       <c r="N5" s="284"/>
       <c r="O5" s="284"/>
       <c r="P5" s="284"/>
-      <c r="Q5" s="309" t="s">
+      <c r="Q5" s="308" t="s">
         <v>311</v>
       </c>
-      <c r="R5" s="309"/>
-      <c r="S5" s="309"/>
-      <c r="T5" s="309"/>
-      <c r="U5" s="309"/>
-      <c r="V5" s="309"/>
-      <c r="W5" s="309"/>
-      <c r="X5" s="307">
+      <c r="R5" s="308"/>
+      <c r="S5" s="308"/>
+      <c r="T5" s="308"/>
+      <c r="U5" s="308"/>
+      <c r="V5" s="308"/>
+      <c r="W5" s="308"/>
+      <c r="X5" s="306">
         <f>+X3+X4</f>
         <v>600</v>
       </c>
-      <c r="Y5" s="307"/>
+      <c r="Y5" s="306"/>
       <c r="Z5" s="186"/>
       <c r="AA5" s="186"/>
     </row>
-    <row r="6" spans="1:30" s="181" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" s="181" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="297" t="s">
         <v>160</v>
       </c>
-      <c r="B6" s="272" t="s">
+      <c r="B6" s="274" t="s">
         <v>157</v>
       </c>
-      <c r="C6" s="308" t="s">
+      <c r="C6" s="307" t="s">
         <v>308</v>
       </c>
-      <c r="D6" s="308"/>
-      <c r="E6" s="308"/>
-      <c r="F6" s="308"/>
-      <c r="G6" s="308"/>
-      <c r="H6" s="306" t="s">
+      <c r="D6" s="307"/>
+      <c r="E6" s="307"/>
+      <c r="F6" s="307"/>
+      <c r="G6" s="307"/>
+      <c r="H6" s="305" t="s">
         <v>353</v>
       </c>
-      <c r="I6" s="306"/>
-      <c r="J6" s="306"/>
-      <c r="K6" s="306"/>
-      <c r="L6" s="306"/>
-      <c r="M6" s="306"/>
-      <c r="N6" s="306"/>
-      <c r="O6" s="306"/>
-      <c r="P6" s="306"/>
-      <c r="Q6" s="306"/>
-      <c r="R6" s="306"/>
-      <c r="S6" s="306"/>
-      <c r="T6" s="306"/>
-      <c r="U6" s="306"/>
-      <c r="V6" s="306"/>
-      <c r="W6" s="306"/>
-      <c r="X6" s="306"/>
-      <c r="Y6" s="306"/>
-      <c r="Z6" s="306"/>
-      <c r="AA6" s="306"/>
-      <c r="AD6" s="181">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" s="181" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="305"/>
+      <c r="J6" s="305"/>
+      <c r="K6" s="305"/>
+      <c r="L6" s="305"/>
+      <c r="M6" s="305"/>
+      <c r="N6" s="305"/>
+      <c r="O6" s="305"/>
+      <c r="P6" s="305"/>
+      <c r="Q6" s="305"/>
+      <c r="R6" s="305"/>
+      <c r="S6" s="305"/>
+      <c r="T6" s="305"/>
+      <c r="U6" s="305"/>
+      <c r="V6" s="305"/>
+      <c r="W6" s="305"/>
+      <c r="X6" s="305"/>
+      <c r="Y6" s="305"/>
+      <c r="Z6" s="305"/>
+      <c r="AA6" s="305"/>
+    </row>
+    <row r="7" spans="1:29" s="181" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="298"/>
-      <c r="B7" s="273"/>
-      <c r="C7" s="273" t="s">
+      <c r="B7" s="275"/>
+      <c r="C7" s="275" t="s">
         <v>354</v>
       </c>
-      <c r="D7" s="273"/>
-      <c r="E7" s="273"/>
-      <c r="F7" s="273"/>
-      <c r="G7" s="273"/>
+      <c r="D7" s="275"/>
+      <c r="E7" s="275"/>
+      <c r="F7" s="275"/>
+      <c r="G7" s="275"/>
       <c r="H7" s="293" t="s">
         <v>369</v>
       </c>
@@ -16475,14 +16464,10 @@
       <c r="Y7" s="294"/>
       <c r="Z7" s="295"/>
       <c r="AA7" s="200"/>
-      <c r="AD7" s="181">
-        <f>+AD6*0.3</f>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" s="181" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:29" s="181" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="298"/>
-      <c r="B8" s="273"/>
+      <c r="B8" s="275"/>
       <c r="C8" s="281" t="s">
         <v>367</v>
       </c>
@@ -16559,49 +16544,49 @@
         <v>349</v>
       </c>
     </row>
-    <row r="9" spans="1:30" s="181" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" s="181" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="298"/>
-      <c r="B9" s="273"/>
+      <c r="B9" s="275"/>
       <c r="C9" s="282"/>
-      <c r="D9" s="305"/>
-      <c r="E9" s="305"/>
-      <c r="F9" s="305"/>
+      <c r="D9" s="304"/>
+      <c r="E9" s="304"/>
+      <c r="F9" s="304"/>
       <c r="G9" s="282"/>
       <c r="H9" s="192" t="s">
         <v>316</v>
       </c>
       <c r="I9" s="192" t="s">
+        <v>385</v>
+      </c>
+      <c r="J9" s="192" t="s">
         <v>386</v>
-      </c>
-      <c r="J9" s="192" t="s">
-        <v>387</v>
       </c>
       <c r="K9" s="192" t="s">
         <v>318</v>
       </c>
       <c r="L9" s="192" t="s">
+        <v>387</v>
+      </c>
+      <c r="M9" s="192" t="s">
         <v>388</v>
       </c>
-      <c r="M9" s="192" t="s">
+      <c r="N9" s="192" t="s">
         <v>389</v>
       </c>
-      <c r="N9" s="192" t="s">
+      <c r="O9" s="192" t="s">
         <v>390</v>
       </c>
-      <c r="O9" s="192" t="s">
+      <c r="P9" s="192" t="s">
         <v>391</v>
       </c>
-      <c r="P9" s="192" t="s">
+      <c r="Q9" s="192" t="s">
         <v>392</v>
       </c>
-      <c r="Q9" s="192" t="s">
+      <c r="R9" s="192" t="s">
         <v>393</v>
       </c>
-      <c r="R9" s="192" t="s">
+      <c r="S9" s="192" t="s">
         <v>394</v>
-      </c>
-      <c r="S9" s="192" t="s">
-        <v>395</v>
       </c>
       <c r="T9" s="192" t="s">
         <v>366</v>
@@ -16628,9 +16613,9 @@
         <v>305</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="181" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" s="181" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="299"/>
-      <c r="B10" s="274"/>
+      <c r="B10" s="276"/>
       <c r="C10" s="283"/>
       <c r="D10" s="195" t="s">
         <v>380</v>
@@ -16699,7 +16684,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="181" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" s="181" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A11" s="205"/>
       <c r="B11" s="201"/>
       <c r="C11" s="202"/>
@@ -16728,7 +16713,7 @@
       <c r="Z11" s="190"/>
       <c r="AA11" s="204"/>
     </row>
-    <row r="12" spans="1:30" s="181" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" s="181" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="206"/>
       <c r="B12" s="207"/>
       <c r="C12" s="208"/>
@@ -16757,16 +16742,13 @@
       <c r="Z12" s="211"/>
       <c r="AA12" s="213"/>
     </row>
-    <row r="13" spans="1:30" s="181" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" s="181" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="217"/>
       <c r="B13" s="218" t="s">
         <v>373</v>
       </c>
       <c r="C13" s="218"/>
-      <c r="D13" s="231">
-        <f>SUM(G11:G115)</f>
-        <v>0</v>
-      </c>
+      <c r="D13" s="231"/>
       <c r="E13" s="218"/>
       <c r="F13" s="285"/>
       <c r="G13" s="285"/>
@@ -16791,7 +16773,7 @@
       <c r="Z13" s="284"/>
       <c r="AA13" s="214"/>
     </row>
-    <row r="14" spans="1:30" s="181" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" s="181" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A14" s="217"/>
       <c r="B14" s="219" t="s">
         <v>376</v>
@@ -16822,7 +16804,7 @@
       <c r="Z14" s="214"/>
       <c r="AA14" s="214"/>
     </row>
-    <row r="15" spans="1:30" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A15" s="217"/>
       <c r="B15" s="220" t="s">
         <v>372</v>
@@ -16853,7 +16835,7 @@
       <c r="Z15" s="216"/>
       <c r="AA15" s="216"/>
     </row>
-    <row r="16" spans="1:30" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A16" s="217"/>
       <c r="B16" s="220" t="s">
         <v>374</v>
@@ -16876,7 +16858,7 @@
       <c r="R16" s="216"/>
       <c r="S16" s="216"/>
       <c r="T16" s="216"/>
-      <c r="U16" s="276"/>
+      <c r="U16" s="277"/>
       <c r="V16" s="277"/>
       <c r="W16" s="277"/>
       <c r="X16" s="277"/>
@@ -16907,11 +16889,11 @@
       <c r="R17" s="216"/>
       <c r="S17" s="216"/>
       <c r="T17" s="216"/>
-      <c r="U17" s="275"/>
-      <c r="V17" s="275"/>
-      <c r="W17" s="275"/>
-      <c r="X17" s="275"/>
-      <c r="Y17" s="275"/>
+      <c r="U17" s="216"/>
+      <c r="V17" s="216"/>
+      <c r="W17" s="216"/>
+      <c r="X17" s="216"/>
+      <c r="Y17" s="216"/>
       <c r="Z17" s="216"/>
       <c r="AA17" s="216"/>
     </row>
@@ -16938,7 +16920,7 @@
       <c r="R18" s="226"/>
       <c r="S18" s="226"/>
       <c r="T18" s="226"/>
-      <c r="U18" s="333"/>
+      <c r="U18" s="232"/>
       <c r="V18" s="226"/>
       <c r="W18" s="226"/>
       <c r="X18" s="226"/>
@@ -16975,8 +16957,12 @@
       <c r="Z19" s="226"/>
       <c r="AA19" s="226"/>
     </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="M20" s="233"/>
+    </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="43">
+    <mergeCell ref="L1:Z1"/>
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="N4:O4"/>
@@ -17001,13 +16987,10 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="P3:W3"/>
     <mergeCell ref="P4:W4"/>
-    <mergeCell ref="L1:S1"/>
-    <mergeCell ref="T1:Z1"/>
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="X4:Y4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="B6:B10"/>
-    <mergeCell ref="U17:Y17"/>
     <mergeCell ref="U16:Y16"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F16:G16"/>
@@ -17078,72 +17061,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315" t="s">
+      <c r="B2" s="314" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="316"/>
-      <c r="D2" s="316"/>
-      <c r="E2" s="316"/>
-      <c r="F2" s="316"/>
-      <c r="G2" s="316"/>
-      <c r="H2" s="316"/>
-      <c r="I2" s="316"/>
-      <c r="J2" s="316"/>
-      <c r="K2" s="316"/>
-      <c r="L2" s="316"/>
-      <c r="M2" s="317"/>
+      <c r="C2" s="315"/>
+      <c r="D2" s="315"/>
+      <c r="E2" s="315"/>
+      <c r="F2" s="315"/>
+      <c r="G2" s="315"/>
+      <c r="H2" s="315"/>
+      <c r="I2" s="315"/>
+      <c r="J2" s="315"/>
+      <c r="K2" s="315"/>
+      <c r="L2" s="315"/>
+      <c r="M2" s="316"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="318" t="s">
+      <c r="B3" s="317" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="320" t="s">
+      <c r="C3" s="319" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="320" t="s">
+      <c r="D3" s="319" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="322" t="s">
+      <c r="E3" s="321" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="324" t="s">
+      <c r="F3" s="323" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="325"/>
-      <c r="H3" s="325"/>
-      <c r="I3" s="325"/>
-      <c r="J3" s="325"/>
-      <c r="K3" s="325"/>
-      <c r="L3" s="325"/>
-      <c r="M3" s="326"/>
+      <c r="G3" s="324"/>
+      <c r="H3" s="324"/>
+      <c r="I3" s="324"/>
+      <c r="J3" s="324"/>
+      <c r="K3" s="324"/>
+      <c r="L3" s="324"/>
+      <c r="M3" s="325"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="319"/>
-      <c r="C4" s="321"/>
-      <c r="D4" s="321"/>
-      <c r="E4" s="323"/>
-      <c r="F4" s="327"/>
-      <c r="G4" s="328"/>
-      <c r="H4" s="328"/>
-      <c r="I4" s="328"/>
-      <c r="J4" s="328"/>
-      <c r="K4" s="328"/>
-      <c r="L4" s="328"/>
-      <c r="M4" s="329"/>
+      <c r="B4" s="318"/>
+      <c r="C4" s="320"/>
+      <c r="D4" s="320"/>
+      <c r="E4" s="322"/>
+      <c r="F4" s="326"/>
+      <c r="G4" s="327"/>
+      <c r="H4" s="327"/>
+      <c r="I4" s="327"/>
+      <c r="J4" s="327"/>
+      <c r="K4" s="327"/>
+      <c r="L4" s="327"/>
+      <c r="M4" s="328"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="314"/>
-      <c r="C5" s="314"/>
-      <c r="D5" s="314"/>
-      <c r="E5" s="314"/>
-      <c r="F5" s="314"/>
-      <c r="G5" s="314"/>
-      <c r="H5" s="314"/>
-      <c r="I5" s="314"/>
-      <c r="J5" s="314"/>
-      <c r="K5" s="314"/>
-      <c r="L5" s="314"/>
-      <c r="M5" s="314"/>
+      <c r="B5" s="313"/>
+      <c r="C5" s="313"/>
+      <c r="D5" s="313"/>
+      <c r="E5" s="313"/>
+      <c r="F5" s="313"/>
+      <c r="G5" s="313"/>
+      <c r="H5" s="313"/>
+      <c r="I5" s="313"/>
+      <c r="J5" s="313"/>
+      <c r="K5" s="313"/>
+      <c r="L5" s="313"/>
+      <c r="M5" s="313"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -17756,72 +17739,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315" t="s">
+      <c r="B2" s="314" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="316"/>
-      <c r="D2" s="316"/>
-      <c r="E2" s="316"/>
-      <c r="F2" s="316"/>
-      <c r="G2" s="316"/>
-      <c r="H2" s="316"/>
-      <c r="I2" s="316"/>
-      <c r="J2" s="316"/>
-      <c r="K2" s="316"/>
-      <c r="L2" s="316"/>
-      <c r="M2" s="317"/>
+      <c r="C2" s="315"/>
+      <c r="D2" s="315"/>
+      <c r="E2" s="315"/>
+      <c r="F2" s="315"/>
+      <c r="G2" s="315"/>
+      <c r="H2" s="315"/>
+      <c r="I2" s="315"/>
+      <c r="J2" s="315"/>
+      <c r="K2" s="315"/>
+      <c r="L2" s="315"/>
+      <c r="M2" s="316"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="318" t="s">
+      <c r="B3" s="317" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="320" t="s">
+      <c r="C3" s="319" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="320" t="s">
+      <c r="D3" s="319" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="322" t="s">
+      <c r="E3" s="321" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="324" t="s">
+      <c r="F3" s="323" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="325"/>
-      <c r="H3" s="325"/>
-      <c r="I3" s="325"/>
-      <c r="J3" s="325"/>
-      <c r="K3" s="325"/>
-      <c r="L3" s="325"/>
-      <c r="M3" s="326"/>
+      <c r="G3" s="324"/>
+      <c r="H3" s="324"/>
+      <c r="I3" s="324"/>
+      <c r="J3" s="324"/>
+      <c r="K3" s="324"/>
+      <c r="L3" s="324"/>
+      <c r="M3" s="325"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="319"/>
-      <c r="C4" s="321"/>
-      <c r="D4" s="321"/>
-      <c r="E4" s="323"/>
-      <c r="F4" s="327"/>
-      <c r="G4" s="328"/>
-      <c r="H4" s="328"/>
-      <c r="I4" s="328"/>
-      <c r="J4" s="328"/>
-      <c r="K4" s="328"/>
-      <c r="L4" s="328"/>
-      <c r="M4" s="329"/>
+      <c r="B4" s="318"/>
+      <c r="C4" s="320"/>
+      <c r="D4" s="320"/>
+      <c r="E4" s="322"/>
+      <c r="F4" s="326"/>
+      <c r="G4" s="327"/>
+      <c r="H4" s="327"/>
+      <c r="I4" s="327"/>
+      <c r="J4" s="327"/>
+      <c r="K4" s="327"/>
+      <c r="L4" s="327"/>
+      <c r="M4" s="328"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="314"/>
-      <c r="C5" s="314"/>
-      <c r="D5" s="314"/>
-      <c r="E5" s="314"/>
-      <c r="F5" s="330"/>
-      <c r="G5" s="330"/>
-      <c r="H5" s="330"/>
-      <c r="I5" s="330"/>
-      <c r="J5" s="330"/>
-      <c r="K5" s="330"/>
-      <c r="L5" s="330"/>
-      <c r="M5" s="330"/>
+      <c r="B5" s="313"/>
+      <c r="C5" s="313"/>
+      <c r="D5" s="313"/>
+      <c r="E5" s="313"/>
+      <c r="F5" s="329"/>
+      <c r="G5" s="329"/>
+      <c r="H5" s="329"/>
+      <c r="I5" s="329"/>
+      <c r="J5" s="329"/>
+      <c r="K5" s="329"/>
+      <c r="L5" s="329"/>
+      <c r="M5" s="329"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -18422,72 +18405,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="315" t="s">
+      <c r="B2" s="314" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="316"/>
-      <c r="D2" s="316"/>
-      <c r="E2" s="316"/>
-      <c r="F2" s="316"/>
-      <c r="G2" s="316"/>
-      <c r="H2" s="316"/>
-      <c r="I2" s="316"/>
-      <c r="J2" s="316"/>
-      <c r="K2" s="316"/>
-      <c r="L2" s="316"/>
-      <c r="M2" s="317"/>
+      <c r="C2" s="315"/>
+      <c r="D2" s="315"/>
+      <c r="E2" s="315"/>
+      <c r="F2" s="315"/>
+      <c r="G2" s="315"/>
+      <c r="H2" s="315"/>
+      <c r="I2" s="315"/>
+      <c r="J2" s="315"/>
+      <c r="K2" s="315"/>
+      <c r="L2" s="315"/>
+      <c r="M2" s="316"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="318" t="s">
+      <c r="B3" s="317" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="320" t="s">
+      <c r="C3" s="319" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="320" t="s">
+      <c r="D3" s="319" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="322" t="s">
+      <c r="E3" s="321" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="324" t="s">
+      <c r="F3" s="323" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="325"/>
-      <c r="H3" s="325"/>
-      <c r="I3" s="325"/>
-      <c r="J3" s="325"/>
-      <c r="K3" s="325"/>
-      <c r="L3" s="325"/>
-      <c r="M3" s="326"/>
+      <c r="G3" s="324"/>
+      <c r="H3" s="324"/>
+      <c r="I3" s="324"/>
+      <c r="J3" s="324"/>
+      <c r="K3" s="324"/>
+      <c r="L3" s="324"/>
+      <c r="M3" s="325"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="319"/>
-      <c r="C4" s="321"/>
-      <c r="D4" s="321"/>
-      <c r="E4" s="323"/>
-      <c r="F4" s="327"/>
-      <c r="G4" s="328"/>
-      <c r="H4" s="328"/>
-      <c r="I4" s="328"/>
-      <c r="J4" s="328"/>
-      <c r="K4" s="328"/>
-      <c r="L4" s="328"/>
-      <c r="M4" s="329"/>
+      <c r="B4" s="318"/>
+      <c r="C4" s="320"/>
+      <c r="D4" s="320"/>
+      <c r="E4" s="322"/>
+      <c r="F4" s="326"/>
+      <c r="G4" s="327"/>
+      <c r="H4" s="327"/>
+      <c r="I4" s="327"/>
+      <c r="J4" s="327"/>
+      <c r="K4" s="327"/>
+      <c r="L4" s="327"/>
+      <c r="M4" s="328"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="331"/>
-      <c r="C5" s="314"/>
-      <c r="D5" s="314"/>
-      <c r="E5" s="314"/>
-      <c r="F5" s="314"/>
-      <c r="G5" s="314"/>
-      <c r="H5" s="314"/>
-      <c r="I5" s="314"/>
-      <c r="J5" s="314"/>
-      <c r="K5" s="314"/>
-      <c r="L5" s="314"/>
-      <c r="M5" s="332"/>
+      <c r="B5" s="330"/>
+      <c r="C5" s="313"/>
+      <c r="D5" s="313"/>
+      <c r="E5" s="313"/>
+      <c r="F5" s="313"/>
+      <c r="G5" s="313"/>
+      <c r="H5" s="313"/>
+      <c r="I5" s="313"/>
+      <c r="J5" s="313"/>
+      <c r="K5" s="313"/>
+      <c r="L5" s="313"/>
+      <c r="M5" s="331"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">

</xml_diff>